<commit_message>
Excel & forecaster.db updated with 3 products 2 services
</commit_message>
<xml_diff>
--- a/ProductHierarchy.xlsx
+++ b/ProductHierarchy.xlsx
@@ -714,7 +714,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,6 +863,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -880,6 +883,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -897,6 +903,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
@@ -914,6 +923,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -931,6 +943,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -948,6 +963,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
New function; organized data after SQLite extraction; modified README.md
</commit_message>
<xml_diff>
--- a/ProductHierarchy.xlsx
+++ b/ProductHierarchy.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="4590" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10773" windowHeight="4593"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>Product</t>
   </si>
@@ -425,17 +425,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.29296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +452,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -469,10 +469,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>1</v>
-      </c>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="C3">
         <v>2</v>
       </c>
@@ -483,10 +480,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>1</v>
-      </c>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="C4">
         <v>3</v>
       </c>
@@ -497,7 +491,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B5">
         <v>2</v>
       </c>
@@ -511,10 +505,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>2</v>
-      </c>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="C6">
         <v>2</v>
       </c>
@@ -525,10 +516,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>2</v>
-      </c>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="C7">
         <v>3</v>
       </c>
@@ -539,7 +527,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -556,7 +544,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -573,14 +561,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
         <v>2</v>
       </c>
       <c r="D10">
@@ -590,7 +572,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -607,10 +589,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>1</v>
-      </c>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="C12">
         <v>2</v>
       </c>
@@ -621,7 +600,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -651,12 +630,12 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -664,7 +643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -672,7 +651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -680,7 +659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -688,7 +667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -696,7 +675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -713,16 +692,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -742,7 +721,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -762,7 +741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -782,7 +761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -802,7 +781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -822,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -842,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -862,7 +841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -882,7 +861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -902,7 +881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -922,7 +901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -942,7 +921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -962,7 +941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>12</v>
       </c>

</xml_diff>